<commit_message>
Interfaces ethernet tests executed after nokia configuration
</commit_message>
<xml_diff>
--- a/AutomationFramework/results/07102020/logs/interfaces_test_if_ethernet_test_if_ethernet_aggregate_id_logs.xlsx
+++ b/AutomationFramework/results/07102020/logs/interfaces_test_if_ethernet_test_if_ethernet_aggregate_id_logs.xlsx
@@ -53,6 +53,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -445,7 +513,7 @@
                     &lt;filter&gt;
                         &lt;interfaces xmlns="http://openconfig.net/yang/interfaces"&gt;
                         &lt;interface&gt;
-                        &lt;name&gt;1/1/c11/2&lt;/name&gt;
+                        &lt;name&gt;1/1/1&lt;/name&gt;
                         &lt;/interface&gt;
                         &lt;/interfaces&gt;
                     &lt;/filter&gt;
@@ -455,24 +523,31 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:a1acb4a3-2c02-48bc-a6de-5991d94230f2" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:746e106d-83da-4bfe-8f4b-9bff3c5d2e3d" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;data&gt;
     &lt;/data&gt;
 &lt;/rpc-reply&gt; 
 -------------------
 &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:995e6a93-489c-4bee-b991-6057e0dcccac" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:dde397d5-a583-4a97-b71f-7b1cd1f29e58" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;data&gt;
         &lt;interfaces xmlns="http://openconfig.net/yang/interfaces"&gt;
             &lt;interface&gt;
-                &lt;name&gt;1/1/c11/2&lt;/name&gt;
+                &lt;name&gt;1/1/1&lt;/name&gt;
                 &lt;config&gt;
-                    &lt;name&gt;1/1/c11/2&lt;/name&gt;
+                    &lt;name&gt;1/1/1&lt;/name&gt;
                     &lt;type&gt;ethernetCsmacd&lt;/type&gt;
                     &lt;mtu&gt;1500&lt;/mtu&gt;
-                    &lt;description&gt;TestSamier 2&lt;/description&gt;
+                    &lt;description&gt;test&lt;/description&gt;
                     &lt;enabled&gt;true&lt;/enabled&gt;
                 &lt;/config&gt;
+                &lt;ethernet xmlns="http://openconfig.net/yang/interfaces/ethernet"&gt;
+                    &lt;config&gt;
+                        &lt;auto-negotiate&gt;false&lt;/auto-negotiate&gt;
+                        &lt;duplex-mode&gt;FULL&lt;/duplex-mode&gt;
+                        &lt;port-speed&gt;SPEED_100MB&lt;/port-speed&gt;
+                    &lt;/config&gt;
+                &lt;/ethernet&gt;
             &lt;/interface&gt;
         &lt;/interfaces&gt;
     &lt;/data&gt;
@@ -506,7 +581,7 @@
     &lt;config&gt;
       &lt;interfaces xmlns="http://openconfig.net/yang/interfaces"&gt;
         &lt;interface&gt;
-          &lt;name&gt;1/1/c11/2&lt;/name&gt;
+          &lt;name&gt;1/1/1&lt;/name&gt;
           &lt;ethernet xmlns="http://openconfig.net/yang/interfaces/ethernet"&gt;
             &lt;config&gt;
               &lt;aggregate-id xmlns="http://openconfig.net/yang/interfaces/aggregate"&gt;lag-1&lt;/aggregate-id&gt;
@@ -521,20 +596,20 @@
       <c r="H2" t="inlineStr">
         <is>
           <t>- Response of edit-config: &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:28a6b6dd-fa05-416a-aad3-1a2a8d57b59b" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:8331c687-afda-4095-9577-1643acc83fa0" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;ok/&gt;
 &lt;/rpc-reply&gt; 
  - Response of commit: &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:6d35f1c3-2d2d-442e-98c7-d51693417ac1" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:f657f7cb-0ab8-49e4-a995-76e30e2a2bec" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;ok/&gt;
 &lt;/rpc-reply&gt; 
 -------------------
 - Response of edit-config: &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:a01f61d7-afcf-464d-ac16-a6d25bba0448" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:130c8d38-d7bb-4460-8a01-3cf030f783e7" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;ok/&gt;
 &lt;/rpc-reply&gt; 
  - Response of commit: &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:9651d3c7-1db9-439b-964c-1cc116cde6ee" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:e1d22199-55bf-4b43-8311-80f09b72deb3" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;ok/&gt;
 &lt;/rpc-reply&gt;</t>
         </is>
@@ -542,7 +617,7 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:30fd390c-633a-43bb-89c3-a1360a4a304c" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:c2d6484d-7f1b-4e11-a381-56e67adbf4bd" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;data&gt;
         &lt;interfaces xmlns="http://openconfig.net/yang/interfaces"&gt;
             &lt;interface&gt;
@@ -558,20 +633,23 @@
 &lt;/rpc-reply&gt; 
 -------------------
 &lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:c06c747d-0e6a-482c-8fe8-b7ad152aaa8c" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+&lt;rpc-reply message-id="urn:uuid:2d61ec01-e33f-4989-a66f-ca004e7426c6" xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0" xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
     &lt;data&gt;
         &lt;interfaces xmlns="http://openconfig.net/yang/interfaces"&gt;
             &lt;interface&gt;
-                &lt;name&gt;1/1/c11/2&lt;/name&gt;
+                &lt;name&gt;1/1/1&lt;/name&gt;
                 &lt;config&gt;
-                    &lt;name&gt;1/1/c11/2&lt;/name&gt;
+                    &lt;name&gt;1/1/1&lt;/name&gt;
                     &lt;type&gt;ethernetCsmacd&lt;/type&gt;
                     &lt;mtu&gt;1500&lt;/mtu&gt;
-                    &lt;description&gt;TestSamier 2&lt;/description&gt;
+                    &lt;description&gt;test&lt;/description&gt;
                     &lt;enabled&gt;true&lt;/enabled&gt;
                 &lt;/config&gt;
                 &lt;ethernet xmlns="http://openconfig.net/yang/interfaces/ethernet"&gt;
                     &lt;config&gt;
+                        &lt;auto-negotiate&gt;false&lt;/auto-negotiate&gt;
+                        &lt;duplex-mode&gt;FULL&lt;/duplex-mode&gt;
+                        &lt;port-speed&gt;SPEED_100MB&lt;/port-speed&gt;
                         &lt;aggregate-id&gt;lag-1&lt;/aggregate-id&gt;
                     &lt;/config&gt;
                 &lt;/ethernet&gt;

</xml_diff>